<commit_message>
Added resolution and tile size to data.
</commit_message>
<xml_diff>
--- a/data/Frame Rates.xlsx
+++ b/data/Frame Rates.xlsx
@@ -613,8 +613,22 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Number of Lights: 1024 - Radius: 10</a:t>
+              <a:t>Number of Lights: 1024 - Radius: 10 - Tile Size: 16 x 16 pixels</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Resolution:</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 1920 x 1080</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>

</xml_diff>